<commit_message>
Moved the ccs files around. Made separaye files for NumericalRef and NameRef. Also updated the surveys.
</commit_message>
<xml_diff>
--- a/Iteration 1/Survey/Survey_v4.xlsx
+++ b/Iteration 1/Survey/Survey_v4.xlsx
@@ -463,18 +463,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -483,7 +483,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -509,12 +508,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,7 +811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q33" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1131,31 +1131,31 @@
       <c r="J48" s="4"/>
     </row>
     <row r="49" spans="1:10" ht="15.75">
-      <c r="A49" s="41" t="s">
+      <c r="A49" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="42" t="s">
+      <c r="B49" s="43"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="E49" s="43"/>
-      <c r="F49" s="49" t="s">
+      <c r="E49" s="45"/>
+      <c r="F49" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="G49" s="50"/>
-      <c r="H49" s="51"/>
-      <c r="I49" s="55" t="s">
+      <c r="G49" s="51"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="J49" s="56"/>
+      <c r="J49" s="57"/>
     </row>
     <row r="50" spans="1:10" ht="34.5" customHeight="1">
-      <c r="A50" s="52"/>
-      <c r="B50" s="40"/>
-      <c r="C50" s="40"/>
-      <c r="D50" s="40"/>
-      <c r="E50" s="38"/>
+      <c r="A50" s="53"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="35"/>
       <c r="F50" s="15" t="s">
         <v>77</v>
       </c>
@@ -1165,33 +1165,33 @@
       <c r="H50" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="I50" s="53" t="s">
+      <c r="I50" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="J50" s="54"/>
+      <c r="J50" s="55"/>
     </row>
     <row r="51" spans="1:10" s="2" customFormat="1" ht="18.75">
-      <c r="A51" s="46" t="s">
+      <c r="A51" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="47"/>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
-      <c r="J51" s="48"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="48"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="48"/>
+      <c r="J51" s="49"/>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="44" t="s">
+      <c r="A52" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="45"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="41"/>
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
@@ -1203,13 +1203,13 @@
       </c>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="39" t="s">
+      <c r="A53" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="40"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="38"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="35"/>
       <c r="F53" s="21"/>
       <c r="G53" s="21"/>
       <c r="H53" s="21"/>
@@ -1221,13 +1221,13 @@
       </c>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="39" t="s">
+      <c r="A54" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B54" s="40"/>
-      <c r="C54" s="38"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="38"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="35"/>
       <c r="F54" s="21"/>
       <c r="G54" s="21"/>
       <c r="H54" s="21"/>
@@ -1239,13 +1239,13 @@
       </c>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="39" t="s">
+      <c r="A55" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B55" s="40"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="38"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="35"/>
       <c r="F55" s="21"/>
       <c r="G55" s="21"/>
       <c r="H55" s="21"/>
@@ -1257,13 +1257,13 @@
       </c>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="39" t="s">
+      <c r="A56" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="40"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="38"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="35"/>
       <c r="F56" s="21"/>
       <c r="G56" s="21"/>
       <c r="H56" s="21"/>
@@ -1275,27 +1275,27 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" customHeight="1">
-      <c r="A57" s="33" t="s">
+      <c r="A57" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="34"/>
-      <c r="C57" s="34"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="35"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="35"/>
+      <c r="B57" s="59"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B58" s="40"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="38"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="60"/>
+      <c r="E58" s="35"/>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -1361,13 +1361,13 @@
       </c>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="39" t="s">
+      <c r="A62" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B62" s="40"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="38"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="60"/>
+      <c r="E62" s="35"/>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
@@ -1382,29 +1382,29 @@
       <c r="A63" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="35"/>
-      <c r="C63" s="35"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="35"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="35"/>
-      <c r="J63" s="35"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="37"/>
+      <c r="G63" s="37"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="37"/>
+      <c r="J63" s="37"/>
     </row>
     <row r="64" spans="1:10" ht="15.75">
-      <c r="A64" s="57" t="s">
+      <c r="A64" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B64" s="58"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="58"/>
-      <c r="E64" s="58"/>
-      <c r="F64" s="58"/>
-      <c r="G64" s="58"/>
-      <c r="H64" s="58"/>
-      <c r="I64" s="58"/>
-      <c r="J64" s="59"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="39"/>
+      <c r="I64" s="39"/>
+      <c r="J64" s="40"/>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="22" t="s">
@@ -1446,28 +1446,28 @@
       <c r="A67" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="35"/>
-      <c r="C67" s="35"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
-      <c r="F67" s="35"/>
-      <c r="G67" s="35"/>
-      <c r="H67" s="35"/>
-      <c r="I67" s="35"/>
-      <c r="J67" s="35"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37"/>
+      <c r="J67" s="37"/>
     </row>
     <row r="68" spans="1:10" ht="15.75">
-      <c r="A68" s="57" t="s">
+      <c r="A68" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="58"/>
-      <c r="C68" s="58"/>
-      <c r="D68" s="58"/>
-      <c r="E68" s="58"/>
-      <c r="F68" s="58"/>
-      <c r="G68" s="58"/>
-      <c r="H68" s="58"/>
-      <c r="I68" s="58"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="39"/>
+      <c r="I68" s="39"/>
       <c r="J68" s="26"/>
     </row>
     <row r="69" spans="1:10">
@@ -1489,13 +1489,13 @@
       </c>
     </row>
     <row r="70" spans="1:10">
-      <c r="A70" s="39" t="s">
+      <c r="A70" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B70" s="40"/>
-      <c r="C70" s="40"/>
-      <c r="D70" s="40"/>
-      <c r="E70" s="38"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="34"/>
+      <c r="E70" s="35"/>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
@@ -1510,24 +1510,24 @@
       <c r="A71" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="B71" s="35"/>
-      <c r="C71" s="35"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
-      <c r="F71" s="35"/>
-      <c r="G71" s="35"/>
-      <c r="H71" s="35"/>
-      <c r="I71" s="35"/>
-      <c r="J71" s="35"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="37"/>
+      <c r="G71" s="37"/>
+      <c r="H71" s="37"/>
+      <c r="I71" s="37"/>
+      <c r="J71" s="37"/>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="39" t="s">
+      <c r="A72" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="B72" s="40"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="45"/>
-      <c r="E72" s="45"/>
+      <c r="B72" s="34"/>
+      <c r="C72" s="35"/>
+      <c r="D72" s="41"/>
+      <c r="E72" s="41"/>
       <c r="F72" s="9"/>
       <c r="G72" s="8"/>
       <c r="H72" s="9"/>
@@ -1539,13 +1539,13 @@
       </c>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="39" t="s">
+      <c r="A73" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B73" s="40"/>
-      <c r="C73" s="38"/>
-      <c r="D73" s="45"/>
-      <c r="E73" s="45"/>
+      <c r="B73" s="34"/>
+      <c r="C73" s="35"/>
+      <c r="D73" s="41"/>
+      <c r="E73" s="41"/>
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
       <c r="H73" s="9"/>
@@ -1636,10 +1636,10 @@
       <c r="H81" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="I81" s="60" t="s">
+      <c r="I81" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="J81" s="60"/>
+      <c r="J81" s="42"/>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="11"/>
@@ -1652,8 +1652,8 @@
       <c r="F82" s="11"/>
       <c r="G82" s="31"/>
       <c r="H82" s="5"/>
-      <c r="I82" s="45"/>
-      <c r="J82" s="45"/>
+      <c r="I82" s="41"/>
+      <c r="J82" s="41"/>
     </row>
     <row r="83" spans="1:10">
       <c r="C83" s="11"/>
@@ -1662,8 +1662,8 @@
       </c>
       <c r="E83" s="1"/>
       <c r="H83" s="5"/>
-      <c r="I83" s="45"/>
-      <c r="J83" s="45"/>
+      <c r="I83" s="41"/>
+      <c r="J83" s="41"/>
     </row>
     <row r="84" spans="1:10">
       <c r="C84" s="11"/>
@@ -1672,8 +1672,8 @@
       </c>
       <c r="E84" s="1"/>
       <c r="H84" s="5"/>
-      <c r="I84" s="45"/>
-      <c r="J84" s="45"/>
+      <c r="I84" s="41"/>
+      <c r="J84" s="41"/>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="1" t="s">
@@ -1797,28 +1797,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A70:E70"/>
-    <mergeCell ref="A67:J67"/>
-    <mergeCell ref="A64:J64"/>
-    <mergeCell ref="A68:I68"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="I81:J81"/>
-    <mergeCell ref="I82:J82"/>
-    <mergeCell ref="A71:J71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="I83:J83"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="A51:J51"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="D52:E52"/>
     <mergeCell ref="A57:J57"/>
     <mergeCell ref="A63:J63"/>
     <mergeCell ref="D56:E56"/>
@@ -1833,11 +1811,33 @@
     <mergeCell ref="A62:C62"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="A51:J51"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="A70:E70"/>
+    <mergeCell ref="A67:J67"/>
+    <mergeCell ref="A64:J64"/>
+    <mergeCell ref="A68:I68"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="I81:J81"/>
+    <mergeCell ref="I82:J82"/>
+    <mergeCell ref="A71:J71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="I83:J83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"-,Bold"&amp;14Navigation survey for voice controlled browsing</oddHeader>
+    <oddHeader>&amp;C&amp;"-,Bold"&amp;14Navigation survey for voice controlled browsing - Iteration 1</oddHeader>
   </headerFooter>
 </worksheet>
 </file>

</xml_diff>